<commit_message>
KORA_S1_P2 adjustments with preliminary files where unclear variables were deleted
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P2.xlsx
+++ b/rmonize/data_schema/Dataschema_P2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\Pilot_Datenharmonisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C5312C1-FF56-41D3-B603-A6C20CC7CA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25A9D7C7-E0B9-445B-8DF1-DA8B736BC9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="243">
   <si>
     <t>index</t>
   </si>
@@ -57,7 +57,7 @@
     <t>variable_ID</t>
   </si>
   <si>
-    <t>participant identification number</t>
+    <t>Participant identification number</t>
   </si>
   <si>
     <t>integer</t>
@@ -162,6 +162,12 @@
     <t>Number of live births given</t>
   </si>
   <si>
+    <t>AGE_FIRST_BIRTH</t>
+  </si>
+  <si>
+    <t>Age at the first given birth</t>
+  </si>
+  <si>
     <t>TG</t>
   </si>
   <si>
@@ -186,9 +192,6 @@
     <t>HDL cholesterol measured from blood samples</t>
   </si>
   <si>
-    <t>AGE_FIRST_BIRTH</t>
-  </si>
-  <si>
     <t>Age at first given birth</t>
   </si>
   <si>
@@ -615,7 +618,7 @@
     <t>SUGAR_CONFECT_11</t>
   </si>
   <si>
-    <t>sugar and confectionary intake [g/d]</t>
+    <t>Intake of sugar and similar, confectionery and water-based sweet desserts [g/d]</t>
   </si>
   <si>
     <t>CAKES_12</t>
@@ -627,61 +630,61 @@
     <t>FRUITVEG_JUICE_1301</t>
   </si>
   <si>
-    <t>fruit and vegetable juice intake [g/d]</t>
+    <t>Intake of fruit and vegetable juices and nectars [g/d]</t>
   </si>
   <si>
     <t>SOFTDRINKS_1302</t>
   </si>
   <si>
-    <t>softdrink intake [g/d]</t>
+    <t>Intake of soft drinks (flavoured, no fruit) [g/d]</t>
   </si>
   <si>
     <t>ART_SWEETENER_170201</t>
   </si>
   <si>
-    <t>artificial sweetener intake [g/d]</t>
+    <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
   </si>
   <si>
     <t>VEGETABLES_02</t>
   </si>
   <si>
-    <t>vegetables intake [g/d]</t>
+    <t>Vegetable intake [g/d]</t>
   </si>
   <si>
     <t>LEGUMES_TOT_03</t>
   </si>
   <si>
-    <t>total legumes intake [g/d]</t>
+    <t>Legumes intake [g/d]</t>
   </si>
   <si>
     <t>FRUITS_TOT_04</t>
   </si>
   <si>
-    <t>total fruit intake [g/d]</t>
+    <t>intake of any type of RPCs of fruit nature [g/d]</t>
   </si>
   <si>
     <t>RED_MEAT_0701</t>
   </si>
   <si>
-    <t>red meat intake [g/d]</t>
+    <t>Intake of red meat (mammals meat) [g/d]</t>
   </si>
   <si>
     <t>PROCMEAT_0704</t>
   </si>
   <si>
-    <t>processed meat intake [g/d]</t>
+    <t>Intake of processed or preserved meat [g/d]</t>
   </si>
   <si>
     <t>COFFEE_130301</t>
   </si>
   <si>
-    <t>coffee intake [g/d]</t>
+    <t>Coffee intake [g/d]</t>
   </si>
   <si>
     <t>TEA_130302</t>
   </si>
   <si>
-    <t>tea intake [g/d]</t>
+    <t>Tea intake [g/d]</t>
   </si>
   <si>
     <t>variable</t>
@@ -772,7 +775,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,6 +855,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -876,7 +885,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -935,6 +944,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1252,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N130"/>
+  <dimension ref="A1:N131"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -1291,7 +1306,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1317,7 +1332,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>7</v>
@@ -1332,7 +1347,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -1345,9 +1360,9 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="4">
-        <v>3</v>
+    <row r="5" spans="1:14" ht="15">
+      <c r="A5" s="3">
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -1362,7 +1377,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>13</v>
@@ -1377,7 +1392,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>15</v>
@@ -1390,9 +1405,9 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="4">
-        <v>6</v>
+    <row r="8" spans="1:14" ht="15">
+      <c r="A8" s="3">
+        <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>17</v>
@@ -1405,9 +1420,9 @@
       </c>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="15">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>20</v>
@@ -1420,9 +1435,9 @@
       </c>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="4">
-        <v>8</v>
+    <row r="10" spans="1:14" ht="15">
+      <c r="A10" s="3">
+        <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>22</v>
@@ -1437,7 +1452,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>24</v>
@@ -1452,7 +1467,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>26</v>
@@ -1465,9 +1480,9 @@
       </c>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="4">
-        <v>11</v>
+    <row r="13" spans="1:14" ht="15">
+      <c r="A13" s="3">
+        <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>28</v>
@@ -1482,7 +1497,7 @@
     </row>
     <row r="14" spans="1:14" ht="29.1">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>30</v>
@@ -1497,7 +1512,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>32</v>
@@ -1510,9 +1525,9 @@
       </c>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="4">
-        <v>14</v>
+    <row r="16" spans="1:14" ht="15">
+      <c r="A16" s="3">
+        <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>34</v>
@@ -1527,7 +1542,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>36</v>
@@ -1540,9 +1555,9 @@
       </c>
       <c r="E17" s="17"/>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4">
-        <v>16</v>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="3">
+        <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>38</v>
@@ -1555,24 +1570,24 @@
       </c>
       <c r="E18" s="17"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="4">
-        <v>17</v>
-      </c>
-      <c r="B19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>42</v>
@@ -1585,9 +1600,9 @@
       </c>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4">
-        <v>19</v>
+    <row r="21" spans="1:5" ht="15">
+      <c r="A21" s="3">
+        <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>44</v>
@@ -1602,7 +1617,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>46</v>
@@ -1617,28 +1632,28 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="4">
-        <v>21</v>
-      </c>
-      <c r="B23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="21" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4">
-        <v>22</v>
+    <row r="24" spans="1:5" ht="15">
+      <c r="A24" s="3">
+        <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>6</v>
@@ -1647,27 +1662,28 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="15">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4">
-        <v>24</v>
-      </c>
-      <c r="B26" s="12" t="s">
+      <c r="C26" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>6</v>
@@ -1675,86 +1691,85 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" ht="29.1">
-      <c r="A28" s="4">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" ht="30.75">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="4" customFormat="1">
-      <c r="A29" s="4">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:5" s="4" customFormat="1">
       <c r="A30" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1" ht="15">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="17"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="4">
-        <v>29</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" spans="1:5" ht="15">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="4">
-        <v>30</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>6</v>
@@ -1763,13 +1778,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>6</v>
@@ -1778,103 +1793,103 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" ht="15">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="18"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="4">
-        <v>33</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5" ht="15">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="18"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="4">
-        <v>35</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="1:5" ht="15">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="17"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="4">
-        <v>36</v>
-      </c>
-      <c r="B38" s="12" t="s">
+      <c r="C38" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="17"/>
-    </row>
-    <row r="39" spans="1:5" ht="29.1">
-      <c r="A39" s="4">
-        <v>37</v>
-      </c>
-      <c r="B39" s="12" t="s">
+      <c r="C39" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="1:5" ht="30.75">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="17"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4">
-        <v>38</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>6</v>
@@ -1883,13 +1898,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>6</v>
@@ -1898,28 +1913,28 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="4">
-        <v>40</v>
-      </c>
-      <c r="B42" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="1:5" ht="15">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="17"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="4">
-        <v>41</v>
-      </c>
-      <c r="B43" s="15" t="s">
+      <c r="C43" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>6</v>
@@ -1928,28 +1943,28 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="4">
-        <v>42</v>
-      </c>
-      <c r="B44" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="17"/>
+    </row>
+    <row r="45" spans="1:5" ht="15">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="17"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="4">
-        <v>43</v>
-      </c>
-      <c r="B45" s="12" t="s">
+      <c r="C45" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>6</v>
@@ -1958,13 +1973,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="4">
-        <v>44</v>
-      </c>
-      <c r="B46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>6</v>
@@ -1973,103 +1988,103 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="17"/>
+    </row>
+    <row r="48" spans="1:5" ht="15">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="48" spans="1:5" ht="29.1">
-      <c r="A48" s="4">
-        <v>46</v>
-      </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="18"/>
+      <c r="E48" s="17"/>
     </row>
     <row r="49" spans="1:5" ht="29.1">
       <c r="A49" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="18"/>
+    </row>
+    <row r="50" spans="1:5" ht="29.1">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="17"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="4">
-        <v>48</v>
-      </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="17"/>
+    </row>
+    <row r="51" spans="1:5" ht="15">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="17"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="4">
-        <v>49</v>
-      </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52" spans="1:5" ht="15">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="17"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="4">
-        <v>50</v>
-      </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="17"/>
+    </row>
+    <row r="53" spans="1:5" ht="15">
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="4">
-        <v>51</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>6</v>
@@ -2078,13 +2093,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>6</v>
@@ -2093,28 +2108,28 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4">
-        <v>53</v>
-      </c>
-      <c r="B55" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="17"/>
+    </row>
+    <row r="56" spans="1:5" ht="15">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="4">
-        <v>54</v>
-      </c>
-      <c r="B56" s="13" t="s">
+      <c r="C56" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>6</v>
@@ -2123,13 +2138,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>6</v>
@@ -2138,28 +2153,28 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4">
-        <v>56</v>
-      </c>
-      <c r="B58" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59" spans="1:5" ht="15">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="17"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="4">
-        <v>57</v>
-      </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>6</v>
@@ -2168,13 +2183,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>6</v>
@@ -2183,550 +2198,682 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="D61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="17"/>
+    </row>
+    <row r="62" spans="1:5" ht="15">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="17"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="4">
-        <v>60</v>
-      </c>
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="D62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="17"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="17"/>
-    </row>
-    <row r="63" spans="1:5" ht="29.1">
-      <c r="A63" s="4">
-        <v>61</v>
-      </c>
-      <c r="B63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="D63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="17"/>
+    </row>
+    <row r="64" spans="1:5" ht="30.75">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="1:5" ht="29.1">
-      <c r="A64" s="4">
-        <v>63</v>
-      </c>
-      <c r="B64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="D64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E64" s="17"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" ht="29.1">
       <c r="A65" s="4">
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66" spans="1:5" ht="15">
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D65" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="B66" s="17" t="s">
+      <c r="C66" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="D66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="1:5" ht="15">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="17"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="B67" s="17" t="s">
+      <c r="C67" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="D67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="17"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4">
+        <v>67</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="18"/>
-    </row>
-    <row r="68" spans="1:5" ht="29.1">
-      <c r="B68" s="17" t="s">
+      <c r="C68" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="D68" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="18"/>
+    </row>
+    <row r="69" spans="1:5" ht="29.1">
+      <c r="A69" s="4">
+        <v>68</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D68" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" spans="1:5" ht="29.1">
-      <c r="B69" s="7" t="s">
+      <c r="C69" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="D69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" spans="1:5" ht="30.75">
+      <c r="A70" s="3">
+        <v>69</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="B70" s="7" t="s">
+      <c r="C70" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4">
+        <v>70</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E70" s="18"/>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="B71" s="7" t="s">
+      <c r="C71" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="18"/>
+    </row>
+    <row r="72" spans="1:5" ht="15">
+      <c r="A72" s="3">
+        <v>71</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="B72" s="7" t="s">
+      <c r="C72" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15">
+      <c r="A73" s="4">
+        <v>72</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="B73" s="7" t="s">
+      <c r="C73" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="D73" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4">
+        <v>73</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="B74" s="7" t="s">
+      <c r="C74" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="D74" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15">
+      <c r="A75" s="3">
+        <v>74</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D74" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="B75" s="7" t="s">
+      <c r="C75" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="B76" s="7" t="s">
+      <c r="C76" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="D76" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4">
+        <v>76</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D76" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="B77" s="7" t="s">
+      <c r="C77" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="D77" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15">
+      <c r="A78" s="3">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D77" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="B78" s="7" t="s">
+      <c r="C78" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="D78" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4">
+        <v>78</v>
+      </c>
+      <c r="B79" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D78" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="B79" s="7" t="s">
+      <c r="C79" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="D79" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D79" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="B80" s="7" t="s">
+      <c r="C80" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="D80" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4">
+        <v>80</v>
+      </c>
+      <c r="B81" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D80" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4">
-      <c r="B81" s="19" t="s">
+      <c r="C81" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="D81" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4">
+        <v>81</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4">
-      <c r="B82" s="7" t="s">
+      <c r="C82" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="D82" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15">
+      <c r="A83" s="3">
+        <v>82</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4">
-      <c r="B83" s="7" t="s">
+      <c r="C83" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="D83" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="4">
+        <v>83</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D83" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4">
-      <c r="B84" s="7" t="s">
+      <c r="C84" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="D84" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="4">
+        <v>84</v>
+      </c>
+      <c r="B85" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4">
-      <c r="B85" s="7" t="s">
+      <c r="C85" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="D85" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15">
+      <c r="A86" s="3">
+        <v>85</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D85" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4">
-      <c r="B86" s="7" t="s">
+      <c r="C86" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="D86" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15">
+      <c r="A87" s="4">
+        <v>86</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D86" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4">
-      <c r="B87" s="7" t="s">
+      <c r="C87" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="D87" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="4">
+        <v>87</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D87" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4">
-      <c r="B88" s="7" t="s">
+      <c r="C88" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="D88" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15">
+      <c r="A89" s="3">
+        <v>88</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4">
-      <c r="B89" s="7" t="s">
+      <c r="C89" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="D89" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="4">
+        <v>89</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4">
-      <c r="B90" s="7" t="s">
+      <c r="C90" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="D90" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15">
+      <c r="A91" s="3">
+        <v>90</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D90" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4">
-      <c r="B91" s="7" t="s">
+      <c r="C91" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="D91" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="4">
+        <v>91</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4">
-      <c r="B92" s="7" t="s">
+      <c r="C92" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="D92" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="4">
+        <v>92</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4">
-      <c r="B93" s="7" t="s">
+      <c r="C93" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="D93" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15">
+      <c r="A94" s="3">
+        <v>93</v>
+      </c>
+      <c r="B94" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4">
-      <c r="B94" s="4" t="s">
+      <c r="C94" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="D94" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30.75">
+      <c r="A95" s="4">
+        <v>94</v>
+      </c>
+      <c r="B95" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4">
-      <c r="B95" s="4" t="s">
+      <c r="C95" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="D95" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15">
+      <c r="A96" s="4">
+        <v>95</v>
+      </c>
+      <c r="B96" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4">
-      <c r="B96" s="4" t="s">
+      <c r="C96" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="D96" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="30.75">
+      <c r="A97" s="3">
+        <v>96</v>
+      </c>
+      <c r="B97" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5">
-      <c r="B97" s="4" t="s">
+      <c r="C97" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="D97" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="30.75">
+      <c r="A98" s="4">
+        <v>97</v>
+      </c>
+      <c r="B98" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="D97" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5">
-      <c r="B98" s="4" t="s">
+      <c r="C98" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="D98" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="30.75">
+      <c r="A99" s="3">
+        <v>98</v>
+      </c>
+      <c r="B99" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5">
-      <c r="B99" s="4" t="s">
+      <c r="C99" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="D99" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15">
+      <c r="A100" s="4">
+        <v>99</v>
+      </c>
+      <c r="B100" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="D99" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E99" s="7"/>
-    </row>
-    <row r="100" spans="2:5">
-      <c r="B100" s="4" t="s">
+      <c r="C100" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="D100" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100" s="7"/>
+    </row>
+    <row r="101" spans="1:5" ht="15">
+      <c r="A101" s="4">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D100" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E100" s="7"/>
-    </row>
-    <row r="101" spans="2:5">
-      <c r="B101" s="4" t="s">
+      <c r="C101" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="D101" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E101" s="7"/>
+    </row>
+    <row r="102" spans="1:5" ht="30.75">
+      <c r="A102" s="3">
+        <v>101</v>
+      </c>
+      <c r="B102" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="D101" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E101" s="7"/>
-    </row>
-    <row r="102" spans="2:5">
-      <c r="B102" s="4" t="s">
+      <c r="C102" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="D102" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E102" s="7"/>
+    </row>
+    <row r="103" spans="1:5" ht="15">
+      <c r="A103" s="4">
+        <v>102</v>
+      </c>
+      <c r="B103" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="D102" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E102" s="19"/>
-    </row>
-    <row r="103" spans="2:5">
-      <c r="B103" s="4" t="s">
+      <c r="C103" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="D103" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E103" s="19"/>
+    </row>
+    <row r="104" spans="1:5" ht="15">
+      <c r="A104" s="4">
+        <v>103</v>
+      </c>
+      <c r="B104" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E103" s="7"/>
-    </row>
-    <row r="104" spans="2:5">
-      <c r="B104" s="4" t="s">
+      <c r="C104" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="D104" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" ht="15">
+      <c r="A105" s="3">
+        <v>104</v>
+      </c>
+      <c r="B105" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E104" s="7"/>
-    </row>
-    <row r="105" spans="2:5">
-      <c r="B105" s="4" t="s">
+      <c r="C105" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="D105" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E105" s="7"/>
+    </row>
+    <row r="106" spans="1:5" ht="15">
+      <c r="A106" s="4">
+        <v>105</v>
+      </c>
+      <c r="B106" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="D105" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E105" s="7"/>
-    </row>
-    <row r="106" spans="2:5">
+      <c r="C106" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>19</v>
+      </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="2:5">
+    <row r="107" spans="1:5">
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="2:5">
+    <row r="108" spans="1:5">
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="2:5">
+    <row r="109" spans="1:5">
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="2:5">
+    <row r="110" spans="1:5">
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="2:5">
+    <row r="111" spans="1:5">
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="2:5">
+    <row r="112" spans="1:5">
       <c r="E112" s="7"/>
     </row>
     <row r="113" spans="5:5">
@@ -2782,6 +2929,9 @@
     </row>
     <row r="130" spans="5:5">
       <c r="E130" s="7"/>
+    </row>
+    <row r="131" spans="5:5">
+      <c r="E131" s="7"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2797,24 +2947,25 @@
     <hyperlink ref="B8" r:id="rId4" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:TOT_PA_QX:Dataschema" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B18" r:id="rId5" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_WH_LIVE_BIRTHS:Dataschema" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B16" r:id="rId6" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_WH_HRT_EVER:Dataschema" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B45" r:id="rId7" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B44" r:id="rId8" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B25" r:id="rId9" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_HYP:Dataschema" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B26" r:id="rId10" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B38" r:id="rId11" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_STAT:Dataschema" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B39" r:id="rId12" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_NSAID:Dataschema" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B24" r:id="rId13" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_DIAB:Dataschema" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B27" r:id="rId14" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B46" r:id="rId7" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B45" r:id="rId8" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B26" r:id="rId9" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_HYP:Dataschema" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B27" r:id="rId10" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B39" r:id="rId11" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_STAT:Dataschema" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B40" r:id="rId12" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_NSAID:Dataschema" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B25" r:id="rId13" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_DIAB:Dataschema" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B28" r:id="rId14" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="B13" r:id="rId15" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:SMOKE_ST:Dataschema" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B23" r:id="rId16" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRH_LIVE_BIRTH_AGE_FIRST:Dataschema" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B24" r:id="rId16" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRH_LIVE_BIRTH_AGE_FIRST:Dataschema" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B6" r:id="rId17" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRK_EMPLOYMENT:Dataschema" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="B14" r:id="rId18" display="https://www.maelstrom-research.org/variable/helti-c-12m-hp:MED_SUPP_VITD_C_12M:Dataschema" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B56" r:id="rId19" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2:Dataschema" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B57" r:id="rId20" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B55" r:id="rId21" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_HF_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B57" r:id="rId19" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2:Dataschema" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B58" r:id="rId20" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B56" r:id="rId21" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_HF_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B19" r:id="rId22" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRH_LIVE_BIRTH_AGE_FIRST:Dataschema" xr:uid="{F95178B2-A127-428C-8F64-5D3549F3A930}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -2822,7 +2973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2834,16 +2985,16 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2851,7 +3002,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2864,7 +3015,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2878,7 +3029,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
@@ -2892,7 +3043,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -2906,7 +3057,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C6" s="11">
         <v>2</v>
@@ -2920,7 +3071,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C7" s="11">
         <v>3</v>
@@ -2934,7 +3085,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C8" s="11">
         <v>4</v>
@@ -2948,7 +3099,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C9" s="11">
         <v>5</v>
@@ -2960,7 +3111,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -2973,7 +3124,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C11" s="11">
         <v>2</v>
@@ -2988,7 +3139,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C12" s="11">
         <v>3</v>
@@ -3003,7 +3154,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C13" s="11">
         <v>4</v>
@@ -3018,7 +3169,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C14" s="11">
         <v>5</v>
@@ -3032,7 +3183,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C15" s="11">
         <v>6</v>
@@ -3046,7 +3197,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C16" s="11">
         <v>7</v>
@@ -3060,7 +3211,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C17" s="11">
         <v>0</v>
@@ -3074,7 +3225,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
@@ -3088,7 +3239,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -3102,7 +3253,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C20" s="11">
         <v>2</v>
@@ -3116,7 +3267,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C21" s="11">
         <v>3</v>
@@ -3130,7 +3281,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C22" s="11">
         <v>4</v>
@@ -3144,7 +3295,7 @@
         <v>30</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C23" s="11">
         <v>0</v>
@@ -3158,7 +3309,7 @@
         <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C24" s="11">
         <v>1</v>
@@ -3171,7 +3322,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C25" s="11">
         <v>0</v>
@@ -3184,7 +3335,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
@@ -3197,7 +3348,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C27" s="11">
         <v>2</v>
@@ -3210,7 +3361,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C28" s="11">
         <v>3</v>
@@ -3223,7 +3374,7 @@
         <v>34</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C29" s="11">
         <v>0</v>
@@ -3236,7 +3387,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C30" s="11">
         <v>1</v>
@@ -3246,10 +3397,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C31" s="11">
         <v>0</v>
@@ -3259,10 +3410,10 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C32" s="11">
         <v>1</v>
@@ -3272,10 +3423,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C33" s="11">
         <v>0</v>
@@ -3285,10 +3436,10 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C34" s="11">
         <v>1</v>
@@ -3298,10 +3449,10 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C35" s="11">
         <v>0</v>
@@ -3311,10 +3462,10 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C36" s="11">
         <v>1</v>
@@ -3324,10 +3475,10 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C37" s="11">
         <v>0</v>
@@ -3337,10 +3488,10 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C38" s="11">
         <v>1</v>
@@ -3348,10 +3499,10 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C39" s="11">
         <v>0</v>
@@ -3359,10 +3510,10 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C40" s="11">
         <v>1</v>
@@ -3370,10 +3521,10 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C41" s="11">
         <v>0</v>
@@ -3381,10 +3532,10 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C42" s="11">
         <v>1</v>
@@ -3392,10 +3543,10 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C43" s="11">
         <v>0</v>
@@ -3403,10 +3554,10 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C44" s="11">
         <v>1</v>
@@ -3414,10 +3565,10 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C45" s="11">
         <v>0</v>
@@ -3425,10 +3576,10 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C46" s="11">
         <v>1</v>
@@ -3436,10 +3587,10 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C47" s="11">
         <v>0</v>
@@ -3447,10 +3598,10 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C48" s="11">
         <v>1</v>
@@ -3458,10 +3609,10 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C49" s="11">
         <v>0</v>
@@ -3469,10 +3620,10 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C50" s="11">
         <v>1</v>
@@ -3480,10 +3631,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C51" s="11">
         <v>0</v>
@@ -3491,10 +3642,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C52" s="11">
         <v>1</v>
@@ -3502,10 +3653,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C53" s="11">
         <v>0</v>
@@ -3513,10 +3664,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C54" s="11">
         <v>1</v>
@@ -3524,10 +3675,10 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C55" s="11">
         <v>0</v>
@@ -3535,10 +3686,10 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C56" s="11">
         <v>1</v>
@@ -3546,10 +3697,10 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C57" s="11">
         <v>0</v>
@@ -3557,10 +3708,10 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C58" s="11">
         <v>1</v>
@@ -3568,10 +3719,10 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C59" s="11">
         <v>0</v>
@@ -3581,10 +3732,10 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C60" s="11">
         <v>1</v>
@@ -3594,10 +3745,10 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C61" s="11">
         <v>0</v>
@@ -3607,10 +3758,10 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C62" s="11">
         <v>1</v>
@@ -3620,10 +3771,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C63" s="11">
         <v>0</v>
@@ -3633,10 +3784,10 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C64" s="11">
         <v>1</v>
@@ -3646,10 +3797,10 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C65" s="11">
         <v>0</v>
@@ -3661,10 +3812,10 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C66" s="11">
         <v>1</v>
@@ -3676,10 +3827,10 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C67" s="11">
         <v>0</v>
@@ -3691,10 +3842,10 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C68" s="11">
         <v>1</v>
@@ -3706,10 +3857,10 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C69" s="11">
         <v>0</v>
@@ -3721,10 +3872,10 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C70" s="11">
         <v>1</v>
@@ -3736,10 +3887,10 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C71" s="11">
         <v>0</v>
@@ -3751,10 +3902,10 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C72" s="11">
         <v>1</v>
@@ -3766,10 +3917,10 @@
     </row>
     <row r="73" spans="1:8" ht="14.1" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C73" s="11">
         <v>0</v>
@@ -3781,10 +3932,10 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C74" s="11">
         <v>1</v>
@@ -3796,10 +3947,10 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C75" s="11">
         <v>0</v>
@@ -3811,10 +3962,10 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C76" s="11">
         <v>1</v>
@@ -3826,10 +3977,10 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C77" s="11">
         <v>0</v>
@@ -3841,10 +3992,10 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C78" s="11">
         <v>1</v>
@@ -3856,10 +4007,10 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C79" s="11">
         <v>0</v>
@@ -3871,10 +4022,10 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C80" s="11">
         <v>1</v>
@@ -3886,10 +4037,10 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C81" s="11">
         <v>0</v>
@@ -3901,10 +4052,10 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C82" s="11">
         <v>1</v>
@@ -3916,10 +4067,10 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C83" s="11">
         <v>0</v>
@@ -3931,10 +4082,10 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C84" s="11">
         <v>1</v>
@@ -3946,10 +4097,10 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C85" s="11">
         <v>0</v>
@@ -3961,10 +4112,10 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C86" s="11">
         <v>1</v>
@@ -3974,10 +4125,10 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C87" s="11">
         <v>0</v>
@@ -3987,10 +4138,10 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C88" s="11">
         <v>1</v>
@@ -4108,27 +4259,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4369,14 +4499,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}"/>
 </file>
</xml_diff>

<commit_message>
changes to P2 documents for KORA
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P2.xlsx
+++ b/rmonize/data_schema/Dataschema_P2.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\Pilot_Datenharmonisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25A9D7C7-E0B9-445B-8DF1-DA8B736BC9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E636D2-52CC-40F2-A1E1-CF1E0E52E8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
-    <sheet name="categories" sheetId="2" r:id="rId2"/>
+    <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
@@ -24,17 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -48,15 +37,9 @@
     <t>name</t>
   </si>
   <si>
-    <t>label:en</t>
-  </si>
-  <si>
     <t>valueType</t>
   </si>
   <si>
-    <t>variable_ID</t>
-  </si>
-  <si>
     <t>Participant identification number</t>
   </si>
   <si>
@@ -192,9 +175,6 @@
     <t>HDL cholesterol measured from blood samples</t>
   </si>
   <si>
-    <t>Age at first given birth</t>
-  </si>
-  <si>
     <t>PREV_DIAB</t>
   </si>
   <si>
@@ -498,13 +478,19 @@
     <t>FMI</t>
   </si>
   <si>
-    <t>Fat mass index at baseline</t>
+    <t>Fat mass index at follow-up</t>
   </si>
   <si>
     <t>BODY_FAT</t>
   </si>
   <si>
-    <t>Body fat at at baseline</t>
+    <t>Body fat at at follow-up</t>
+  </si>
+  <si>
+    <t>AGE_ANTH_FUP</t>
+  </si>
+  <si>
+    <t>Age at anthropometric measurement at follow-up</t>
   </si>
   <si>
     <t>ENERGY</t>
@@ -690,9 +676,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>missing</t>
   </si>
   <si>
@@ -769,13 +752,19 @@
   </si>
   <si>
     <t>surgical postmenopausal (bilateral ovariectomy)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,7 +874,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -950,6 +939,13 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -971,7 +967,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1269,11 +1265,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="34.140625" style="4" bestFit="1" customWidth="1"/>
@@ -1282,7 +1278,7 @@
     <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1290,10 +1286,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="1"/>
@@ -1306,18 +1302,18 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="15">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1"/>
@@ -1330,1607 +1326,1606 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" ht="15">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:14" ht="15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" ht="15">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:14" ht="29.1">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" ht="15">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E18" s="17"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="17" t="s">
+      <c r="D20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" ht="15">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="17" t="s">
+      <c r="D21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C22" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>47</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E22" s="17"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E24" s="17"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" ht="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="12" t="s">
+      <c r="C28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="4" customFormat="1" ht="30.75">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="4" customFormat="1">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E30" s="17"/>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" ht="15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E31" s="17"/>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E32" s="17"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="1:5" ht="15">
-      <c r="A35" s="3">
-        <v>34</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="18"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="4">
-        <v>35</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="17"/>
-    </row>
-    <row r="37" spans="1:5" ht="15">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:5" ht="15">
-      <c r="A38" s="4">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D38" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E38" s="17"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E39" s="17"/>
     </row>
-    <row r="40" spans="1:5" ht="30.75">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="D40" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E40" s="17"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="4">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="17"/>
-    </row>
-    <row r="43" spans="1:5" ht="15">
-      <c r="A43" s="3">
-        <v>42</v>
-      </c>
-      <c r="B43" s="15" t="s">
+      <c r="C43" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="17"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="4">
-        <v>43</v>
-      </c>
-      <c r="B44" s="15" t="s">
+      <c r="C44" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="17"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="17"/>
-    </row>
-    <row r="45" spans="1:5" ht="15">
-      <c r="A45" s="3">
-        <v>44</v>
-      </c>
-      <c r="B45" s="12" t="s">
+      <c r="C45" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="4">
-        <v>45</v>
-      </c>
-      <c r="B46" s="12" t="s">
+      <c r="C46" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E46" s="17"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E47" s="17"/>
     </row>
-    <row r="48" spans="1:5" ht="15">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="D48" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:5" ht="29.1">
+        <v>4</v>
+      </c>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="17"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="18"/>
-    </row>
-    <row r="50" spans="1:5" ht="29.1">
-      <c r="A50" s="4">
-        <v>49</v>
-      </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="17"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="17"/>
-    </row>
-    <row r="51" spans="1:5" ht="15">
-      <c r="A51" s="3">
-        <v>50</v>
-      </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="17"/>
-    </row>
-    <row r="52" spans="1:5" ht="15">
-      <c r="A52" s="4">
-        <v>51</v>
-      </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="17"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="1:5" ht="15">
-      <c r="A53" s="3">
-        <v>52</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="D53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="17"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="4">
-        <v>53</v>
-      </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="D54" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E54" s="17"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D55" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E55" s="17"/>
     </row>
-    <row r="56" spans="1:5" ht="15">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="D56" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E56" s="17"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="17"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="17"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="4">
-        <v>57</v>
-      </c>
-      <c r="B58" s="13" t="s">
+      <c r="C58" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="17"/>
-    </row>
-    <row r="59" spans="1:5" ht="15">
-      <c r="A59" s="3">
-        <v>58</v>
-      </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="17"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="17"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="4">
-        <v>59</v>
-      </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D60" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E60" s="17"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="D61" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E61" s="17"/>
     </row>
-    <row r="62" spans="1:5" ht="15">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="D62" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E62" s="17"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="D63" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E63" s="17"/>
     </row>
-    <row r="64" spans="1:5" ht="30.75">
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="D64" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E64" s="17"/>
     </row>
-    <row r="65" spans="1:5" ht="29.1">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D65" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="1:5" ht="15">
-      <c r="A66" s="4">
-        <v>65</v>
-      </c>
-      <c r="B66" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>66</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" s="17"/>
-    </row>
-    <row r="67" spans="1:5" ht="15">
-      <c r="A67" s="3">
-        <v>66</v>
-      </c>
-      <c r="B67" s="17" t="s">
+      <c r="C67" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="D67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>67</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="4">
-        <v>67</v>
-      </c>
-      <c r="B68" s="17" t="s">
+      <c r="C68" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="D68" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="18"/>
-    </row>
-    <row r="69" spans="1:5" ht="29.1">
+        <v>17</v>
+      </c>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="20" t="s">
-        <v>140</v>
-      </c>
       <c r="D69" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E69" s="17"/>
     </row>
-    <row r="70" spans="1:5" ht="30.75">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="20" t="s">
-        <v>142</v>
-      </c>
       <c r="D70" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:5">
+        <v>17</v>
+      </c>
+      <c r="E70" s="18"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="D71" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E71" s="18"/>
-    </row>
-    <row r="72" spans="1:5" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="D72" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="D73" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>73</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="4">
-        <v>73</v>
-      </c>
-      <c r="B74" s="7" t="s">
+      <c r="C74" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="D74" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>74</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D74" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15">
-      <c r="A75" s="3">
-        <v>74</v>
-      </c>
-      <c r="B75" s="7" t="s">
+      <c r="C75" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="4">
-        <v>75</v>
-      </c>
-      <c r="B76" s="7" t="s">
+      <c r="C76" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="D76" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="D77" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="D78" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="D79" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="D80" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="D81" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>81</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="4">
-        <v>81</v>
-      </c>
-      <c r="B82" s="19" t="s">
+      <c r="C82" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="D82" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>82</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15">
-      <c r="A83" s="3">
-        <v>82</v>
-      </c>
-      <c r="B83" s="7" t="s">
+      <c r="C83" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="D83" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D83" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="4">
-        <v>83</v>
-      </c>
-      <c r="B84" s="7" t="s">
+      <c r="C84" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>170</v>
-      </c>
       <c r="D84" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>172</v>
-      </c>
       <c r="D85" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="D86" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="D87" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>87</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D87" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="4">
-        <v>87</v>
-      </c>
-      <c r="B88" s="7" t="s">
+      <c r="C88" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="D88" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>88</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15">
-      <c r="A89" s="3">
-        <v>88</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="C89" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="D89" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>89</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="4">
-        <v>89</v>
-      </c>
-      <c r="B90" s="7" t="s">
+      <c r="C90" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="D90" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>90</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D90" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15">
-      <c r="A91" s="3">
-        <v>90</v>
-      </c>
-      <c r="B91" s="7" t="s">
+      <c r="C91" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="D91" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>91</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="4">
-        <v>91</v>
-      </c>
-      <c r="B92" s="7" t="s">
+      <c r="C92" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D92" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="D93" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C94" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="D94" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="30.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>94</v>
       </c>
       <c r="B95" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="C95" s="27" t="s">
+      <c r="D95" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>95</v>
+      </c>
+      <c r="B96" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="D95" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15">
-      <c r="A96" s="4">
-        <v>95</v>
-      </c>
-      <c r="B96" s="26" t="s">
+      <c r="C96" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="C96" s="27" t="s">
+      <c r="D96" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>96</v>
+      </c>
+      <c r="B97" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="D96" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30.75">
-      <c r="A97" s="3">
-        <v>96</v>
-      </c>
-      <c r="B97" s="26" t="s">
+      <c r="C97" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="C97" s="27" t="s">
+      <c r="D97" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>97</v>
+      </c>
+      <c r="B98" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="D97" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="30.75">
-      <c r="A98" s="4">
-        <v>97</v>
-      </c>
-      <c r="B98" s="26" t="s">
+      <c r="C98" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="C98" s="27" t="s">
+      <c r="D98" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>98</v>
+      </c>
+      <c r="B99" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D98" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="30.75">
-      <c r="A99" s="3">
-        <v>98</v>
-      </c>
-      <c r="B99" s="26" t="s">
+      <c r="C99" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="C99" s="27" t="s">
+      <c r="D99" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <v>99</v>
+      </c>
+      <c r="B100" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="D99" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15">
-      <c r="A100" s="4">
-        <v>99</v>
-      </c>
-      <c r="B100" s="26" t="s">
+      <c r="C100" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="C100" s="27" t="s">
-        <v>202</v>
-      </c>
       <c r="D100" s="28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="15">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="D101" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" ht="30.75">
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
       <c r="B102" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C102" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="C102" s="27" t="s">
-        <v>206</v>
-      </c>
       <c r="D102" s="28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" ht="15">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>102</v>
       </c>
       <c r="B103" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C103" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="C103" s="27" t="s">
+      <c r="D103" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" s="19"/>
+    </row>
+    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>103</v>
+      </c>
+      <c r="B104" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="D103" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E103" s="19"/>
-    </row>
-    <row r="104" spans="1:5" ht="15">
-      <c r="A104" s="4">
-        <v>103</v>
-      </c>
-      <c r="B104" s="26" t="s">
+      <c r="C104" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="C104" s="27" t="s">
+      <c r="D104" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>104</v>
+      </c>
+      <c r="B105" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D104" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E104" s="7"/>
-    </row>
-    <row r="105" spans="1:5" ht="15">
-      <c r="A105" s="3">
-        <v>104</v>
-      </c>
-      <c r="B105" s="26" t="s">
+      <c r="C105" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="C105" s="27" t="s">
+      <c r="D105" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E105" s="7"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>105</v>
+      </c>
+      <c r="B106" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="D105" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E105" s="7"/>
-    </row>
-    <row r="106" spans="1:5" ht="15">
-      <c r="A106" s="4">
-        <v>105</v>
-      </c>
-      <c r="B106" s="26" t="s">
+      <c r="C106" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="C106" s="27" t="s">
-        <v>214</v>
-      </c>
       <c r="D106" s="28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="5:5">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="5:5">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="5:5">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="5:5">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="5:5">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="5:5">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="5:5">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="5:5">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="5:5">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="5:5">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="5:5">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="5:5">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="5:5">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="5:5">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="5:5">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="5:5">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="5:5">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="5:5">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="5:5">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="7"/>
     </row>
   </sheetData>
@@ -2947,62 +2942,61 @@
     <hyperlink ref="B8" r:id="rId4" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:TOT_PA_QX:Dataschema" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B18" r:id="rId5" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_WH_LIVE_BIRTHS:Dataschema" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B16" r:id="rId6" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_WH_HRT_EVER:Dataschema" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B46" r:id="rId7" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B45" r:id="rId8" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B26" r:id="rId9" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_HYP:Dataschema" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B27" r:id="rId10" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B39" r:id="rId11" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_STAT:Dataschema" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B40" r:id="rId12" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_NSAID:Dataschema" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B25" r:id="rId13" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_DIAB:Dataschema" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B28" r:id="rId14" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B45" r:id="rId7" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B44" r:id="rId8" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_MI_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B25" r:id="rId9" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_HYP:Dataschema" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B26" r:id="rId10" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B38" r:id="rId11" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_STAT:Dataschema" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B39" r:id="rId12" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:MED_NSAID:Dataschema" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B24" r:id="rId13" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_DIAB:Dataschema" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B27" r:id="rId14" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:PREV_CVD:Dataschema" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="B13" r:id="rId15" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:SMOKE_ST:Dataschema" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B24" r:id="rId16" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRH_LIVE_BIRTH_AGE_FIRST:Dataschema" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B6" r:id="rId17" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRK_EMPLOYMENT:Dataschema" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B14" r:id="rId18" display="https://www.maelstrom-research.org/variable/helti-c-12m-hp:MED_SUPP_VITD_C_12M:Dataschema" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B57" r:id="rId19" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2:Dataschema" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B58" r:id="rId20" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B56" r:id="rId21" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_HF_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B19" r:id="rId22" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRH_LIVE_BIRTH_AGE_FIRST:Dataschema" xr:uid="{F95178B2-A127-428C-8F64-5D3549F3A930}"/>
+    <hyperlink ref="B6" r:id="rId16" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRK_EMPLOYMENT:Dataschema" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B14" r:id="rId17" display="https://www.maelstrom-research.org/variable/helti-c-12m-hp:MED_SUPP_VITD_C_12M:Dataschema" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B56" r:id="rId18" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2:Dataschema" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B57" r:id="rId19" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_DIAB_TYPE2_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B55" r:id="rId20" display="https://www.maelstrom-research.org/variable/canpath-f1-hrfq-hp:F1_DIS_HF_AGE:Dataschema" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B19" r:id="rId21" display="https://www.maelstrom-research.org/variable/chpt-qual-hp:WRH_LIVE_BIRTH_AGE_FIRST:Dataschema" xr:uid="{F95178B2-A127-428C-8F64-5D3549F3A930}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="B10" sqref="B10:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="D1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3010,12 +3004,12 @@
       <c r="G2" s="5"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3024,12 +3018,12 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
@@ -3038,12 +3032,12 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -3052,12 +3046,12 @@
       <c r="G5" s="16"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" s="11">
         <v>2</v>
@@ -3066,12 +3060,12 @@
       <c r="G6" s="4"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C7" s="11">
         <v>3</v>
@@ -3080,12 +3074,12 @@
       <c r="G7" s="16"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C8" s="11">
         <v>4</v>
@@ -3094,24 +3088,24 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C9" s="11">
         <v>5</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -3119,12 +3113,12 @@
       <c r="D10" s="8"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C11" s="11">
         <v>2</v>
@@ -3134,12 +3128,12 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C12" s="11">
         <v>3</v>
@@ -3149,12 +3143,12 @@
       <c r="G12" s="16"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C13" s="11">
         <v>4</v>
@@ -3164,12 +3158,12 @@
       <c r="G13" s="16"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C14" s="11">
         <v>5</v>
@@ -3178,12 +3172,12 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C15" s="11">
         <v>6</v>
@@ -3192,12 +3186,12 @@
       <c r="G15" s="16"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C16" s="11">
         <v>7</v>
@@ -3206,40 +3200,40 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C17" s="11">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" s="32">
         <v>0</v>
       </c>
       <c r="D17" s="8"/>
       <c r="G17" s="16"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="11">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="32">
         <v>1</v>
       </c>
       <c r="D18" s="8"/>
       <c r="G18" s="16"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -3248,12 +3242,12 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C20" s="11">
         <v>2</v>
@@ -3262,12 +3256,12 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C21" s="11">
         <v>3</v>
@@ -3276,12 +3270,12 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C22" s="11">
         <v>4</v>
@@ -3290,12 +3284,12 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C23" s="11">
         <v>0</v>
@@ -3304,12 +3298,12 @@
       <c r="G23" s="16"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C24" s="11">
         <v>1</v>
@@ -3317,12 +3311,12 @@
       <c r="G24" s="16"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C25" s="11">
         <v>0</v>
@@ -3330,12 +3324,12 @@
       <c r="G25" s="16"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
@@ -3343,12 +3337,12 @@
       <c r="G26" s="16"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C27" s="11">
         <v>2</v>
@@ -3356,12 +3350,12 @@
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C28" s="11">
         <v>3</v>
@@ -3369,12 +3363,12 @@
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C29" s="11">
         <v>0</v>
@@ -3382,12 +3376,12 @@
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C30" s="11">
         <v>1</v>
@@ -3395,12 +3389,12 @@
       <c r="G30" s="4"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C31" s="11">
         <v>0</v>
@@ -3408,12 +3402,12 @@
       <c r="G31" s="4"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C32" s="11">
         <v>1</v>
@@ -3421,12 +3415,12 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C33" s="11">
         <v>0</v>
@@ -3434,12 +3428,12 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C34" s="11">
         <v>1</v>
@@ -3447,12 +3441,12 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C35" s="11">
         <v>0</v>
@@ -3460,12 +3454,12 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C36" s="11">
         <v>1</v>
@@ -3473,12 +3467,12 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C37" s="11">
         <v>0</v>
@@ -3486,243 +3480,243 @@
       <c r="G37" s="16"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C38" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C39" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C40" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C41" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C42" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C43" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C44" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C45" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C46" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C47" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C48" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C49" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C50" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C51" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C52" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C53" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C54" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C55" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C56" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C57" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C58" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C59" s="11">
         <v>0</v>
@@ -3730,12 +3724,12 @@
       <c r="E59" s="16"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C60" s="11">
         <v>1</v>
@@ -3743,12 +3737,12 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C61" s="11">
         <v>0</v>
@@ -3756,12 +3750,12 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C62" s="11">
         <v>1</v>
@@ -3769,12 +3763,12 @@
       <c r="E62" s="24"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C63" s="11">
         <v>0</v>
@@ -3782,12 +3776,12 @@
       <c r="E63" s="24"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C64" s="11">
         <v>1</v>
@@ -3795,12 +3789,12 @@
       <c r="E64" s="16"/>
       <c r="F64" s="25"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C65" s="11">
         <v>0</v>
@@ -3810,12 +3804,12 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C66" s="11">
         <v>1</v>
@@ -3825,12 +3819,12 @@
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C67" s="11">
         <v>0</v>
@@ -3840,12 +3834,12 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C68" s="11">
         <v>1</v>
@@ -3855,12 +3849,12 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C69" s="11">
         <v>0</v>
@@ -3870,12 +3864,12 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C70" s="11">
         <v>1</v>
@@ -3885,12 +3879,12 @@
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C71" s="11">
         <v>0</v>
@@ -3900,12 +3894,12 @@
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C72" s="11">
         <v>1</v>
@@ -3915,12 +3909,12 @@
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73" spans="1:8" ht="14.1" customHeight="1">
+    <row r="73" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C73" s="11">
         <v>0</v>
@@ -3930,12 +3924,12 @@
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C74" s="11">
         <v>1</v>
@@ -3945,12 +3939,12 @@
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C75" s="11">
         <v>0</v>
@@ -3960,12 +3954,12 @@
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C76" s="11">
         <v>1</v>
@@ -3975,12 +3969,12 @@
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C77" s="11">
         <v>0</v>
@@ -3990,12 +3984,12 @@
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C78" s="11">
         <v>1</v>
@@ -4005,12 +3999,12 @@
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C79" s="11">
         <v>0</v>
@@ -4020,12 +4014,12 @@
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C80" s="11">
         <v>1</v>
@@ -4035,12 +4029,12 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C81" s="11">
         <v>0</v>
@@ -4050,12 +4044,12 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C82" s="11">
         <v>1</v>
@@ -4065,12 +4059,12 @@
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C83" s="11">
         <v>0</v>
@@ -4080,12 +4074,12 @@
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C84" s="11">
         <v>1</v>
@@ -4095,12 +4089,12 @@
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C85" s="11">
         <v>0</v>
@@ -4110,12 +4104,12 @@
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C86" s="11">
         <v>1</v>
@@ -4123,12 +4117,12 @@
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C87" s="11">
         <v>0</v>
@@ -4136,82 +4130,18 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C88" s="11">
         <v>1</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-    </row>
-    <row r="97" spans="7:8">
-      <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
-    </row>
-    <row r="98" spans="7:8">
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-    </row>
-    <row r="99" spans="7:8">
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-    </row>
-    <row r="100" spans="7:8">
-      <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
-    </row>
-    <row r="101" spans="7:8">
-      <c r="G101" s="7"/>
-      <c r="H101" s="7"/>
-    </row>
-    <row r="102" spans="7:8">
-      <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
-    </row>
-    <row r="103" spans="7:8">
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
-    </row>
-    <row r="104" spans="7:8">
-      <c r="G104" s="7"/>
-      <c r="H104" s="7"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -4259,6 +4189,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4499,7 +4438,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -4511,23 +4450,40 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixing lexical errors p2
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P2.xlsx
+++ b/rmonize/data_schema/Dataschema_P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0297F0-E5E8-49D9-9473-9EEF96807D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09658E2-1D10-4E76-8CA4-4680D4F6CFE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>CONTRACEPTIVE</t>
   </si>
   <si>
-    <t xml:space="preserve">Use of contraceptive pills or injections </t>
-  </si>
-  <si>
     <t>LIVE_BIRTHS</t>
   </si>
   <si>
@@ -250,21 +247,12 @@
     <t>MELANOMA_SCREEN</t>
   </si>
   <si>
-    <t>Screening, Skin cancer</t>
-  </si>
-  <si>
     <t>MAMMO_SCREEN</t>
   </si>
   <si>
-    <t>Screening, Mammography</t>
-  </si>
-  <si>
     <t>CERVICAL_SCREEN</t>
   </si>
   <si>
-    <t>Cervical screening, smear test</t>
-  </si>
-  <si>
     <t>MED_STAT</t>
   </si>
   <si>
@@ -436,27 +424,15 @@
     <t>BMI</t>
   </si>
   <si>
-    <t>Body Mass index at baseline</t>
-  </si>
-  <si>
     <t>BMI_FUP</t>
   </si>
   <si>
-    <t>Body Mass index at follow-up</t>
-  </si>
-  <si>
     <t>BMI_SDS</t>
   </si>
   <si>
-    <t>Body Mass index Standard Deviation Score at baseline (children studies)</t>
-  </si>
-  <si>
     <t>BMI_SDS_FUP</t>
   </si>
   <si>
-    <t>Body Mass index Standard Deviation Score at follow-up (children studies)</t>
-  </si>
-  <si>
     <t>WAIST_FUP</t>
   </si>
   <si>
@@ -496,15 +472,9 @@
     <t>BODY_FAT_FUP</t>
   </si>
   <si>
-    <t>Body fat precent at at follow-up</t>
-  </si>
-  <si>
     <t>BODY_FAT</t>
   </si>
   <si>
-    <t>Body fat precent at at baseline</t>
-  </si>
-  <si>
     <t>AGE_ANTH_FUP</t>
   </si>
   <si>
@@ -604,9 +574,6 @@
     <t>GL</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily glycaemic load </t>
-  </si>
-  <si>
     <t>SODIUM</t>
   </si>
   <si>
@@ -664,9 +631,6 @@
     <t>FRUITS_TOT_04</t>
   </si>
   <si>
-    <t>intake of any type of RPCs of fruit nature [g/d]</t>
-  </si>
-  <si>
     <t>RED_MEAT_0701</t>
   </si>
   <si>
@@ -775,12 +739,6 @@
     <t>FPQ (Food propensity questionnair without portion sizes)</t>
   </si>
   <si>
-    <t>FFQ (Food frequency questionnaire</t>
-  </si>
-  <si>
-    <t>24HDR (24-h dietary recall</t>
-  </si>
-  <si>
     <t>3_d_FR_w (3-day weighing food record)</t>
   </si>
   <si>
@@ -790,10 +748,52 @@
     <t>7_d_FR_w (7-day weighing food record)</t>
   </si>
   <si>
-    <t>24HFL_FFQ (24-h short food list combined with FFQ</t>
+    <t>Intake of any type of RPCs of fruit nature [g/d]</t>
+  </si>
+  <si>
+    <t>Use of contraceptive pills or injections</t>
+  </si>
+  <si>
+    <t>Daily glycaemic load</t>
+  </si>
+  <si>
+    <t>Body fat precent at follow-up</t>
+  </si>
+  <si>
+    <t>Body fat precent at baseline</t>
+  </si>
+  <si>
+    <t>Screening, skin cancer</t>
+  </si>
+  <si>
+    <t>Screening, mammography</t>
+  </si>
+  <si>
+    <t>Screening cervical, smear test</t>
+  </si>
+  <si>
+    <t>Body Mass Index at baseline</t>
+  </si>
+  <si>
+    <t>Body Mass Index at follow-up</t>
+  </si>
+  <si>
+    <t>Body Mass Index Standard Deviation Score at baseline (children studies)</t>
+  </si>
+  <si>
+    <t>Body Mass Index Standard Deviation Score at follow-up (children studies)</t>
   </si>
   <si>
     <t>Dietary Assessment Instrument</t>
+  </si>
+  <si>
+    <t>FFQ (Food frequency questionnaire)</t>
+  </si>
+  <si>
+    <t>24HFL_FFQ (24-h short food list combined with FFQ)</t>
+  </si>
+  <si>
+    <t>24HDR (24-h dietary recall)</t>
   </si>
 </sst>
 </file>
@@ -847,9 +847,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -865,7 +865,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1163,19 +1163,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="C88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375"/>
-    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1407,1295 +1407,1295 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="C24" t="s">
-        <v>51</v>
-      </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
         <v>58</v>
       </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
       </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s">
-        <v>67</v>
-      </c>
       <c r="D32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
         <v>70</v>
       </c>
-      <c r="C34" t="s">
-        <v>71</v>
-      </c>
       <c r="D34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>244</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>245</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>246</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C58" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C65" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>247</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>248</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C69" t="s">
-        <v>141</v>
+        <v>250</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C74" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>243</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C78" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D78" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C80" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D80" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C81" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C83" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C84" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C85" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C86" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C87" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C88" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C89" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C90" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C91" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C92" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C93" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C94" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="D94" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C95" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D95" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C96" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D96" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C97" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D97" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C98" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D98" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C99" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C100" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C101" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D101" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C102" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C103" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D103" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C104" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="D104" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C105" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D105" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C106" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D106" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C107" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D107" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C108" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D108" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="C109" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
@@ -2718,19 +2718,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:C95"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2739,1032 +2739,1032 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B72" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B73" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B74" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B75" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B83" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B85" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B86" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B87" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B88" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B89" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B90" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B91" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C91">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B92" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C92">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B93" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C93">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B94" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C94">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B95" t="s">
         <v>253</v>
@@ -4110,10 +4110,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to Dataschema P2 to include units in the labels of continuous variables and TYPE_CANCER to text
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P2.xlsx
+++ b/rmonize/data_schema/Dataschema_P2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78639753-4B06-4F45-B1D0-02681233C542}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{78639753-4B06-4F45-B1D0-02681233C542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB7696BF-A240-4FCB-9C03-5AB1D9DE5791}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="256">
   <si>
     <t>index</t>
   </si>
@@ -61,7 +72,7 @@
     <t>AGE_BASE</t>
   </si>
   <si>
-    <t>Age at exposure measure</t>
+    <t>Age at exposure measure [years]</t>
   </si>
   <si>
     <t>decimal</t>
@@ -88,13 +99,13 @@
     <t>TOT_PA_QX</t>
   </si>
   <si>
-    <t>Physical activity from questionnaire data</t>
+    <t>Physical activity from questionnaire data [MET-hr/day]</t>
   </si>
   <si>
     <t>TOT_PA_AC</t>
   </si>
   <si>
-    <t>Physical activity from accelerometry data</t>
+    <t>Physical activity from accelerometry data [MET-hr/day]</t>
   </si>
   <si>
     <t>SMOKE_ST</t>
@@ -106,19 +117,19 @@
     <t>TOBACCO_PY</t>
   </si>
   <si>
-    <t>Cumulative lifetime tobacco exposure</t>
+    <t>Cumulative lifetime tobacco exposure  [pack years]</t>
   </si>
   <si>
     <t>TOBACCO_D</t>
   </si>
   <si>
-    <t>Amount of daily tobacco smoked</t>
+    <t>Amount of daily tobacco smoked [g/day]</t>
   </si>
   <si>
     <t>AGE_SMOKE_QUIT</t>
   </si>
   <si>
-    <t>Age at time of quitting smoking</t>
+    <t>Age at time of quitting smoking [years]</t>
   </si>
   <si>
     <t>MED_SUPPL</t>
@@ -142,40 +153,43 @@
     <t>CONTRACEPTIVE</t>
   </si>
   <si>
+    <t>Use of contraceptive pills or injections [years]</t>
+  </si>
+  <si>
     <t>LIVE_BIRTHS</t>
   </si>
   <si>
-    <t>Number of live births given</t>
+    <t>Number of live births given [Nr. of birth]</t>
   </si>
   <si>
     <t>AGE_FIRST_BIRTH</t>
   </si>
   <si>
-    <t>Age at the first given birth</t>
+    <t>Age at the first given birth [years]</t>
   </si>
   <si>
     <t>TG</t>
   </si>
   <si>
-    <t>Triglycerides measured from blood samples</t>
+    <t>Triglycerides measured from blood samples [mmol/L]</t>
   </si>
   <si>
     <t>CHOL</t>
   </si>
   <si>
-    <t>Total cholesterol measured from blood samples</t>
+    <t>Total cholesterol measured from blood samples [mmol/L]</t>
   </si>
   <si>
     <t>LDL</t>
   </si>
   <si>
-    <t>LDL cholesterol measured from blood samples</t>
+    <t>LDL cholesterol measured from blood samples [mmol/L]</t>
   </si>
   <si>
     <t>HDL</t>
   </si>
   <si>
-    <t>HDL cholesterol measured from blood samples</t>
+    <t>HDL cholesterol measured from blood samples [mmol/L]</t>
   </si>
   <si>
     <t>PREV_DIAB</t>
@@ -247,12 +261,21 @@
     <t>MELANOMA_SCREEN</t>
   </si>
   <si>
+    <t>Screening, skin cancer</t>
+  </si>
+  <si>
     <t>MAMMO_SCREEN</t>
   </si>
   <si>
+    <t>Screening, mammography</t>
+  </si>
+  <si>
     <t>CERVICAL_SCREEN</t>
   </si>
   <si>
+    <t>Screening cervical, smear test</t>
+  </si>
+  <si>
     <t>MED_STAT</t>
   </si>
   <si>
@@ -382,7 +405,10 @@
     <t>TYPE_CANCER</t>
   </si>
   <si>
-    <t>Type of Cancer (ICD 10, 3 digits,e.g. C18)</t>
+    <t>Type of Cancer (ICD 10, 3 digits,e.g. C18.3)</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
   <si>
     <t>AGE_CANCER</t>
@@ -418,67 +444,85 @@
     <t>AGE_FUP</t>
   </si>
   <si>
-    <t>Age at end of follow-up</t>
+    <t>Age at end of follow-up [years]</t>
   </si>
   <si>
     <t>BMI</t>
   </si>
   <si>
+    <t>Body Mass Index at baseline [kg/m²]</t>
+  </si>
+  <si>
     <t>BMI_FUP</t>
   </si>
   <si>
+    <t>Body Mass Index at follow-up [kg/m²]</t>
+  </si>
+  <si>
     <t>BMI_SDS</t>
   </si>
   <si>
+    <t>Body Mass Index Standard Deviation Score at baseline (children studies)</t>
+  </si>
+  <si>
     <t>BMI_SDS_FUP</t>
   </si>
   <si>
+    <t>Body Mass Index Standard Deviation Score at follow-up (children studies)</t>
+  </si>
+  <si>
     <t>WAIST_FUP</t>
   </si>
   <si>
-    <t>Waist circumference at follow-up</t>
+    <t>Waist circumference at follow-up [cm]</t>
   </si>
   <si>
     <t>WAIST</t>
   </si>
   <si>
-    <t>Waist circumference at baseline</t>
+    <t>Waist circumference at baseline [cm]</t>
   </si>
   <si>
     <t>HIP</t>
   </si>
   <si>
-    <t>Hip circumference at baseline</t>
+    <t>Hip circumference at baseline [cm]</t>
   </si>
   <si>
     <t>HIP_FUP</t>
   </si>
   <si>
-    <t>Hip circumference at follow-up</t>
+    <t>Hip circumference at follow-up [cm]</t>
   </si>
   <si>
     <t>FMI_FUP</t>
   </si>
   <si>
-    <t>Fat mass index at follow-up</t>
+    <t>Fat mass index at follow-up  [kg/m²]</t>
   </si>
   <si>
     <t>FMI</t>
   </si>
   <si>
-    <t>Fat mass index at baseline</t>
+    <t>Fat mass index at baseline  [kg/m²]</t>
   </si>
   <si>
     <t>BODY_FAT_FUP</t>
   </si>
   <si>
+    <t>Body fat precent at follow-up [%]</t>
+  </si>
+  <si>
     <t>BODY_FAT</t>
   </si>
   <si>
+    <t>Body fat precent at baseline  [%]</t>
+  </si>
+  <si>
     <t>AGE_ANTH_FUP</t>
   </si>
   <si>
-    <t>Age at anthropometric measurement at follow-up</t>
+    <t>Age at anthropometric measurement at follow-up [years]</t>
   </si>
   <si>
     <t>ENERGY</t>
@@ -574,6 +618,9 @@
     <t>GL</t>
   </si>
   <si>
+    <t>Daily glycaemic load</t>
+  </si>
+  <si>
     <t>SODIUM</t>
   </si>
   <si>
@@ -595,12 +642,21 @@
     <t>CAKES_12</t>
   </si>
   <si>
+    <t>Intake of cakes and fine bakery products [g/d]</t>
+  </si>
+  <si>
     <t>FRUITVEG_JUICE_1301</t>
   </si>
   <si>
+    <t>Intake of fruit and vegetable juices [g/d]</t>
+  </si>
+  <si>
     <t>SOFTDRINKS_1302</t>
   </si>
   <si>
+    <t>Intake of soft drinks [g/d]</t>
+  </si>
+  <si>
     <t>ART_SWEETENER_170201</t>
   </si>
   <si>
@@ -616,9 +672,15 @@
     <t>LEGUMES_TOT_03</t>
   </si>
   <si>
+    <t>Total legumes intake [g/d]</t>
+  </si>
+  <si>
     <t>FRUITS_TOT_04</t>
   </si>
   <si>
+    <t>Total fruit intake [g/d]</t>
+  </si>
+  <si>
     <t>RED_MEAT_0701</t>
   </si>
   <si>
@@ -643,6 +705,12 @@
     <t>Tea intake [g/d]</t>
   </si>
   <si>
+    <t>DIETARY_ASSESS_INSTR</t>
+  </si>
+  <si>
+    <t>Dietary Assessment Instrument</t>
+  </si>
+  <si>
     <t>variable</t>
   </si>
   <si>
@@ -721,12 +789,15 @@
     <t>surgical postmenopausal (bilateral ovariectomy)</t>
   </si>
   <si>
-    <t>DIETARY_ASSESS_INSTR</t>
-  </si>
-  <si>
     <t>FPQ (Food propensity questionnair without portion sizes)</t>
   </si>
   <si>
+    <t>FFQ (Food frequency questionnaire)</t>
+  </si>
+  <si>
+    <t>24HDR (24-h dietary recall)</t>
+  </si>
+  <si>
     <t>3_d_FR_w (3-day weighing food record)</t>
   </si>
   <si>
@@ -736,71 +807,14 @@
     <t>7_d_FR_w (7-day weighing food record)</t>
   </si>
   <si>
-    <t>Use of contraceptive pills or injections</t>
-  </si>
-  <si>
-    <t>Daily glycaemic load</t>
-  </si>
-  <si>
-    <t>Body fat precent at follow-up</t>
-  </si>
-  <si>
-    <t>Body fat precent at baseline</t>
-  </si>
-  <si>
-    <t>Screening, skin cancer</t>
-  </si>
-  <si>
-    <t>Screening, mammography</t>
-  </si>
-  <si>
-    <t>Screening cervical, smear test</t>
-  </si>
-  <si>
-    <t>Body Mass Index at baseline</t>
-  </si>
-  <si>
-    <t>Body Mass Index at follow-up</t>
-  </si>
-  <si>
-    <t>Body Mass Index Standard Deviation Score at baseline (children studies)</t>
-  </si>
-  <si>
-    <t>Body Mass Index Standard Deviation Score at follow-up (children studies)</t>
-  </si>
-  <si>
-    <t>Dietary Assessment Instrument</t>
-  </si>
-  <si>
-    <t>FFQ (Food frequency questionnaire)</t>
-  </si>
-  <si>
     <t>24HFL_FFQ (24-h short food list combined with FFQ)</t>
-  </si>
-  <si>
-    <t>24HDR (24-h dietary recall)</t>
-  </si>
-  <si>
-    <t>Intake of cakes and fine bakery products [g/d]</t>
-  </si>
-  <si>
-    <t>Intake of fruit and vegetable juices [g/d]</t>
-  </si>
-  <si>
-    <t>Intake of soft drinks [g/d]</t>
-  </si>
-  <si>
-    <t>Total legumes intake [g/d]</t>
-  </si>
-  <si>
-    <t>Total fruit intake [g/d]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,9 +861,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -865,7 +879,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1163,19 +1177,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C109"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="9.109375"/>
-    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1203,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1217,7 +1231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1245,7 +1259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1259,7 +1273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1273,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1301,7 +1315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1329,7 +1343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1343,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1357,7 +1371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1371,7 +1385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1385,7 +1399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1399,7 +1413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1407,1295 +1421,1295 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>239</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>240</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C65" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>242</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>243</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>244</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>245</v>
+        <v>142</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C72" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C74" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C75" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C76" t="s">
-        <v>237</v>
+        <v>156</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C77" t="s">
-        <v>238</v>
+        <v>158</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="D78" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C79" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="D80" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C81" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C82" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C83" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C84" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C85" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C87" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C88" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="C89" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C90" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C91" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="D92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="C93" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="C94" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="D94" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="D95" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="C96" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="D96" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C97" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="D97" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C98" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D98" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="C99" t="s">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="C100" t="s">
-        <v>252</v>
+        <v>204</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="C101" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="D101" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="C102" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="C103" t="s">
-        <v>253</v>
+        <v>210</v>
       </c>
       <c r="D103" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="C104" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="D104" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C105" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="D105" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C106" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="D106" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="C107" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="D107" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C108" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="D108" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C109" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
@@ -2718,19 +2732,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2739,1035 +2753,1035 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="C15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B53" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B61" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B65" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B68" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B70" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="14.1" customHeight="1">
       <c r="A73" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B77" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B79" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B80" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B82" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B84" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B85" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B86" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B87" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B88" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B89" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B90" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B91" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C91">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B92" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="C92">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B93" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="C93">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B94" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="C94">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B95" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="C95">
         <v>6</v>
@@ -4081,45 +4095,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF9BFE8-2871-49B3-BE95-0B4E5470472F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6DE760F-0358-41C5-A1E3-01D33F9154C5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}"/>
 </file>
</xml_diff>